<commit_message>
Alterações realizadas nas mensagens
</commit_message>
<xml_diff>
--- a/github/files/lista.xlsx
+++ b/github/files/lista.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="340" yWindow="2540" windowWidth="34420" windowHeight="14540"/>
+    <workbookView xWindow="340" yWindow="740" windowWidth="37540" windowHeight="18180"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="372">
   <si>
     <t>Claudino</t>
   </si>
@@ -1082,10 +1082,70 @@
     <t>LINK</t>
   </si>
   <si>
-    <t>http://institucionalteste/evento-criciuma-2017/index.html?368,</t>
-  </si>
-  <si>
     <t>DEFAULT</t>
+  </si>
+  <si>
+    <t>Ana Gracielle</t>
+  </si>
+  <si>
+    <t>Yeda Borgato</t>
+  </si>
+  <si>
+    <t>Ana Gracielilda</t>
+  </si>
+  <si>
+    <t>Yeda Borgato ME</t>
+  </si>
+  <si>
+    <t>anagracielle@focustextil.com.br</t>
+  </si>
+  <si>
+    <t>yedaborgato@focustextil.com.br</t>
+  </si>
+  <si>
+    <t>3522-1895</t>
+  </si>
+  <si>
+    <t>3522-1896</t>
+  </si>
+  <si>
+    <t>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,</t>
+  </si>
+  <si>
+    <t>Claudino de Pellegrin</t>
+  </si>
+  <si>
+    <t>repreclaudino@gmail.com</t>
+  </si>
+  <si>
+    <t>3522-1897</t>
+  </si>
+  <si>
+    <t>3522-1898</t>
+  </si>
+  <si>
+    <t>Luiz José Candido Teixeira Filho</t>
+  </si>
+  <si>
+    <t>luizfilho.ltf@gmail.com</t>
+  </si>
+  <si>
+    <t>Luiz Alberto Carvalho</t>
+  </si>
+  <si>
+    <t>hi.tecidos@gmail.com</t>
+  </si>
+  <si>
+    <t>3522-1899</t>
+  </si>
+  <si>
+    <t>3522-1900</t>
+  </si>
+  <si>
+    <t>Elaine Santos</t>
+  </si>
+  <si>
+    <t>Elaine@focustextil.com.br</t>
   </si>
 </sst>
 </file>
@@ -1166,7 +1226,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1188,6 +1248,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1499,23 +1562,23 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J120"/>
+  <dimension ref="A1:J128"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="50.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="34.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="8.83203125" style="1"/>
     <col min="9" max="9" width="56.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="53" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="57.5" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -1545,7 +1608,7 @@
         <v>348</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>349</v>
@@ -1577,11 +1640,11 @@
         <v>137</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J2" s="4" t="str">
         <f>(I2&amp;""&amp;A2)</f>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1113782473</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1113782473</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1610,11 +1673,11 @@
         <v>137</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J3" s="4" t="str">
         <f>(I3&amp;""&amp;A3)</f>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1158467151</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1158467151</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1643,11 +1706,11 @@
         <v>137</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J4" s="4" t="str">
         <f t="shared" ref="J4:J67" si="0">(I4&amp;""&amp;A4)</f>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1193391625</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1193391625</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1676,11 +1739,11 @@
         <v>138</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J5" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1205478716</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1205478716</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1709,11 +1772,11 @@
         <v>138</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J6" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1244730327</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1244730327</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1742,11 +1805,11 @@
         <v>138</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1263236644</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1263236644</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1775,11 +1838,11 @@
         <v>138</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J8" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1309147825</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1309147825</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1808,11 +1871,11 @@
         <v>139</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J9" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1357282797</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1357282797</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1841,11 +1904,11 @@
         <v>139</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1418644426</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1418644426</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1874,11 +1937,11 @@
         <v>139</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J11" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1490280315</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1490280315</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1907,11 +1970,11 @@
         <v>140</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J12" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1495892863</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1495892863</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1940,11 +2003,11 @@
         <v>140</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1507193617</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1507193617</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1973,11 +2036,11 @@
         <v>140</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1511803637</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1511803637</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2006,11 +2069,11 @@
         <v>141</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1511856644</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1511856644</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2039,11 +2102,11 @@
         <v>142</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1527602566</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1527602566</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2072,11 +2135,11 @@
         <v>142</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J17" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1588804517</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1588804517</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2105,11 +2168,11 @@
         <v>143</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J18" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1633154492</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1633154492</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2138,11 +2201,11 @@
         <v>144</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J19" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1669767734</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1669767734</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2171,11 +2234,11 @@
         <v>144</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J20" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1688737246</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1688737246</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2204,11 +2267,11 @@
         <v>145</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J21" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1734260785</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1734260785</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2237,11 +2300,11 @@
         <v>146</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J22" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1930588703</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1930588703</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2270,11 +2333,11 @@
         <v>146</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J23" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1948180031</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1948180031</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2303,11 +2366,11 @@
         <v>147</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J24" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1957458127</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1957458127</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2336,11 +2399,11 @@
         <v>147</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J25" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1036813484</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1036813484</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2369,11 +2432,11 @@
         <v>148</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J26" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1097884197</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1097884197</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2402,11 +2465,11 @@
         <v>148</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J27" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1104899544</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1104899544</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2435,11 +2498,11 @@
         <v>149</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J28" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1127482178</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1127482178</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2468,11 +2531,11 @@
         <v>149</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J29" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1280570781</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1280570781</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2501,11 +2564,11 @@
         <v>150</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J30" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1300854478</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1300854478</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2534,11 +2597,11 @@
         <v>150</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J31" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1386558404</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1386558404</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2567,11 +2630,11 @@
         <v>151</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J32" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1501706969</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1501706969</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2600,11 +2663,11 @@
         <v>151</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J33" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1503602379</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1503602379</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2633,11 +2696,11 @@
         <v>32</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J34" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1504473445</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1504473445</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2667,11 +2730,11 @@
         <v>32</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J35" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1520358577</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1520358577</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2701,11 +2764,11 @@
         <v>32</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J36" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1586317502</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1586317502</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2735,11 +2798,11 @@
         <v>32</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J37" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1600551988</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1600551988</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2768,11 +2831,11 @@
         <v>33</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J38" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1626677239</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1626677239</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2801,11 +2864,11 @@
         <v>33</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J39" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1630571496</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1630571496</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2834,11 +2897,11 @@
         <v>33</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J40" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1649726488</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1649726488</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2867,11 +2930,11 @@
         <v>34</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J41" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1660484027</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1660484027</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2900,11 +2963,11 @@
         <v>34</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J42" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1667563136</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1667563136</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2933,11 +2996,11 @@
         <v>34</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J43" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1710008438</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1710008438</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2966,11 +3029,11 @@
         <v>35</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J44" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1725406499</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1725406499</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2999,11 +3062,11 @@
         <v>35</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J45" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1749002861</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1749002861</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3032,11 +3095,11 @@
         <v>35</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J46" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1775189048</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1775189048</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3065,11 +3128,11 @@
         <v>36</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J47" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1809503089</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1809503089</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3098,11 +3161,11 @@
         <v>36</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J48" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1814377736</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1814377736</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3131,11 +3194,11 @@
         <v>103</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J49" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1866433814</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1866433814</v>
       </c>
     </row>
     <row r="50" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3164,11 +3227,11 @@
         <v>103</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J50" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1877351355</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1877351355</v>
       </c>
     </row>
     <row r="51" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3197,11 +3260,11 @@
         <v>103</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J51" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1888387868</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1888387868</v>
       </c>
     </row>
     <row r="52" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3230,11 +3293,11 @@
         <v>37</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J52" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,1972015359</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,1972015359</v>
       </c>
     </row>
     <row r="53" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3263,11 +3326,11 @@
         <v>38</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J53" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,2040273348</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,2040273348</v>
       </c>
     </row>
     <row r="54" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3296,11 +3359,11 @@
         <v>38</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J54" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,2061574044</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,2061574044</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3329,11 +3392,11 @@
         <v>39</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J55" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,2070122634</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,2070122634</v>
       </c>
     </row>
     <row r="56" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3362,11 +3425,11 @@
         <v>39</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J56" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,2072884669</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,2072884669</v>
       </c>
     </row>
     <row r="57" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3395,11 +3458,11 @@
         <v>39</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J57" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,2159937988</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,2159937988</v>
       </c>
     </row>
     <row r="58" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3428,11 +3491,11 @@
         <v>40</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J58" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,2177860406</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,2177860406</v>
       </c>
     </row>
     <row r="59" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3461,11 +3524,11 @@
         <v>40</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J59" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,2229172381</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,2229172381</v>
       </c>
     </row>
     <row r="60" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3494,11 +3557,11 @@
         <v>41</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J60" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,2263147174</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,2263147174</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3527,11 +3590,11 @@
         <v>42</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J61" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,2269421526</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,2269421526</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3560,11 +3623,11 @@
         <v>43</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J62" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,2273922832</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,2273922832</v>
       </c>
     </row>
     <row r="63" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3593,11 +3656,11 @@
         <v>43</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J63" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,2296236277</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,2296236277</v>
       </c>
     </row>
     <row r="64" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3626,11 +3689,11 @@
         <v>44</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J64" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,2349994662</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,2349994662</v>
       </c>
     </row>
     <row r="65" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3659,11 +3722,11 @@
         <v>44</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J65" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,2493796813</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,2493796813</v>
       </c>
     </row>
     <row r="66" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3692,11 +3755,11 @@
         <v>44</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J66" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,2495454705</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,2495454705</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3725,11 +3788,11 @@
         <v>45</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J67" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,2527975398</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,2527975398</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3758,11 +3821,11 @@
         <v>46</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J68" s="4" t="str">
-        <f t="shared" ref="J68:J120" si="2">(I68&amp;""&amp;A68)</f>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,2582980564</v>
+        <f t="shared" ref="J68:J126" si="2">(I68&amp;""&amp;A68)</f>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,2582980564</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3791,11 +3854,11 @@
         <v>47</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J69" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,2653933484</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,2653933484</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3824,11 +3887,11 @@
         <v>48</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J70" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,2659726504</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,2659726504</v>
       </c>
     </row>
     <row r="71" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3857,11 +3920,11 @@
         <v>49</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J71" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,2729607097</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,2729607097</v>
       </c>
     </row>
     <row r="72" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3890,11 +3953,11 @@
         <v>49</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J72" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,2735082139</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,2735082139</v>
       </c>
     </row>
     <row r="73" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3923,11 +3986,11 @@
         <v>50</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J73" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,2765266918</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,2765266918</v>
       </c>
     </row>
     <row r="74" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3956,11 +4019,11 @@
         <v>50</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J74" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3077688619</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3077688619</v>
       </c>
     </row>
     <row r="75" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3989,11 +4052,11 @@
         <v>51</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J75" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3085372271</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3085372271</v>
       </c>
     </row>
     <row r="76" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4022,11 +4085,11 @@
         <v>52</v>
       </c>
       <c r="I76" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J76" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3146868713</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3146868713</v>
       </c>
     </row>
     <row r="77" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4055,11 +4118,11 @@
         <v>53</v>
       </c>
       <c r="I77" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J77" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3167047369</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3167047369</v>
       </c>
     </row>
     <row r="78" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4088,11 +4151,11 @@
         <v>53</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J78" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3168971989</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3168971989</v>
       </c>
     </row>
     <row r="79" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4121,11 +4184,11 @@
         <v>54</v>
       </c>
       <c r="I79" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J79" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3196831006</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3196831006</v>
       </c>
     </row>
     <row r="80" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4154,11 +4217,11 @@
         <v>54</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J80" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3213925647</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3213925647</v>
       </c>
     </row>
     <row r="81" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4187,11 +4250,11 @@
         <v>55</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J81" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3294783439</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3294783439</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4220,11 +4283,11 @@
         <v>55</v>
       </c>
       <c r="I82" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J82" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3319564383</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3319564383</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4253,11 +4316,11 @@
         <v>56</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J83" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3338161394</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3338161394</v>
       </c>
     </row>
     <row r="84" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4286,11 +4349,11 @@
         <v>340</v>
       </c>
       <c r="I84" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J84" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3360968144</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3360968144</v>
       </c>
     </row>
     <row r="85" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4319,11 +4382,11 @@
         <v>340</v>
       </c>
       <c r="I85" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J85" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3442296794</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3442296794</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4352,11 +4415,11 @@
         <v>57</v>
       </c>
       <c r="I86" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J86" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3488089461</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3488089461</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4385,11 +4448,11 @@
         <v>58</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J87" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3507353466</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3507353466</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4418,11 +4481,11 @@
         <v>59</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J88" s="4" t="str">
-        <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3570180152</v>
+        <f>(I88&amp;""&amp;A88)</f>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3570180152</v>
       </c>
     </row>
     <row r="89" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4451,11 +4514,11 @@
         <v>60</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J89" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3662490324</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3662490324</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4484,11 +4547,11 @@
         <v>60</v>
       </c>
       <c r="I90" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J90" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3673763304</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3673763304</v>
       </c>
     </row>
     <row r="91" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4517,11 +4580,11 @@
         <v>61</v>
       </c>
       <c r="I91" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J91" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3724961348</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3724961348</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4550,11 +4613,11 @@
         <v>62</v>
       </c>
       <c r="I92" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J92" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3761401901</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3761401901</v>
       </c>
     </row>
     <row r="93" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4583,11 +4646,11 @@
         <v>341</v>
       </c>
       <c r="I93" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J93" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3779049342</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3779049342</v>
       </c>
     </row>
     <row r="94" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4616,11 +4679,11 @@
         <v>341</v>
       </c>
       <c r="I94" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J94" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3830936543</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3830936543</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4649,11 +4712,11 @@
         <v>63</v>
       </c>
       <c r="I95" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J95" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3839920193</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3839920193</v>
       </c>
     </row>
     <row r="96" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4682,11 +4745,11 @@
         <v>63</v>
       </c>
       <c r="I96" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J96" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3873133857</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3873133857</v>
       </c>
     </row>
     <row r="97" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4715,11 +4778,11 @@
         <v>64</v>
       </c>
       <c r="I97" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J97" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3879095929</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3879095929</v>
       </c>
     </row>
     <row r="98" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4748,11 +4811,11 @@
         <v>64</v>
       </c>
       <c r="I98" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J98" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3898209162</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3898209162</v>
       </c>
     </row>
     <row r="99" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4781,11 +4844,11 @@
         <v>65</v>
       </c>
       <c r="I99" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J99" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3957352677</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3957352677</v>
       </c>
     </row>
     <row r="100" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4814,11 +4877,11 @@
         <v>65</v>
       </c>
       <c r="I100" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J100" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,3969217288</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,3969217288</v>
       </c>
     </row>
     <row r="101" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4847,11 +4910,11 @@
         <v>65</v>
       </c>
       <c r="I101" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J101" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,4076996279</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,4076996279</v>
       </c>
     </row>
     <row r="102" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4880,11 +4943,11 @@
         <v>66</v>
       </c>
       <c r="I102" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J102" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,4094882079</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,4094882079</v>
       </c>
     </row>
     <row r="103" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4913,11 +4976,11 @@
         <v>66</v>
       </c>
       <c r="I103" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J103" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,4099973832</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,4099973832</v>
       </c>
     </row>
     <row r="104" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4946,11 +5009,11 @@
         <v>67</v>
       </c>
       <c r="I104" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J104" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,4174348625</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,4174348625</v>
       </c>
     </row>
     <row r="105" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -4979,11 +5042,11 @@
         <v>68</v>
       </c>
       <c r="I105" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J105" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,4221943075</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,4221943075</v>
       </c>
     </row>
     <row r="106" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5012,11 +5075,11 @@
         <v>68</v>
       </c>
       <c r="I106" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J106" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,4281230304</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,4281230304</v>
       </c>
     </row>
     <row r="107" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5045,11 +5108,11 @@
         <v>69</v>
       </c>
       <c r="I107" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J107" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,4293002945</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,4293002945</v>
       </c>
     </row>
     <row r="108" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5078,11 +5141,11 @@
         <v>69</v>
       </c>
       <c r="I108" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J108" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,4316056505</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,4316056505</v>
       </c>
     </row>
     <row r="109" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5111,11 +5174,11 @@
         <v>69</v>
       </c>
       <c r="I109" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J109" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,4320354218</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,4320354218</v>
       </c>
     </row>
     <row r="110" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5144,11 +5207,11 @@
         <v>70</v>
       </c>
       <c r="I110" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J110" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,4334485954</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,4334485954</v>
       </c>
     </row>
     <row r="111" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5177,11 +5240,11 @@
         <v>70</v>
       </c>
       <c r="I111" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J111" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,4343910431</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,4343910431</v>
       </c>
     </row>
     <row r="112" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5210,11 +5273,11 @@
         <v>71</v>
       </c>
       <c r="I112" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J112" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,4368565092</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,4368565092</v>
       </c>
     </row>
     <row r="113" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5243,11 +5306,11 @@
         <v>71</v>
       </c>
       <c r="I113" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J113" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,4376275525</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,4376275525</v>
       </c>
     </row>
     <row r="114" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5276,11 +5339,11 @@
         <v>71</v>
       </c>
       <c r="I114" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J114" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,4396477091</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,4396477091</v>
       </c>
     </row>
     <row r="115" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5309,11 +5372,11 @@
         <v>72</v>
       </c>
       <c r="I115" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J115" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,4541316524</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,4541316524</v>
       </c>
     </row>
     <row r="116" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5342,11 +5405,11 @@
         <v>73</v>
       </c>
       <c r="I116" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J116" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,4558297113</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,4558297113</v>
       </c>
     </row>
     <row r="117" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5375,11 +5438,11 @@
         <v>73</v>
       </c>
       <c r="I117" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J117" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,4612425998</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,4612425998</v>
       </c>
     </row>
     <row r="118" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5408,11 +5471,11 @@
         <v>74</v>
       </c>
       <c r="I118" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J118" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,4628227342</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,4628227342</v>
       </c>
     </row>
     <row r="119" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5441,11 +5504,11 @@
         <v>74</v>
       </c>
       <c r="I119" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J119" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,4704669054</v>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,4704669054</v>
       </c>
     </row>
     <row r="120" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5474,19 +5537,219 @@
         <v>75</v>
       </c>
       <c r="I120" s="4" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
       <c r="J120" s="4" t="str">
         <f t="shared" si="2"/>
-        <v>http://institucionalteste/evento-criciuma-2017/index.html?368,4829606868</v>
-      </c>
-    </row>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,4829606868</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="3">
+        <v>4877613113</v>
+      </c>
+      <c r="B121" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="C121" s="5">
+        <v>1384967000</v>
+      </c>
+      <c r="D121" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="E121" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="F121" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="G121" s="4">
+        <v>11</v>
+      </c>
+      <c r="H121" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="I121" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="J121" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,4877613113</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="3">
+        <v>4914211065</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="C122" s="5">
+        <v>1384967000</v>
+      </c>
+      <c r="D122" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="E122" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="F122" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="G122" s="4">
+        <v>11</v>
+      </c>
+      <c r="H122" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="I122" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="J122" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,4914211065</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="3">
+        <v>4935313154</v>
+      </c>
+      <c r="B123" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="C123" s="5">
+        <v>8888888888</v>
+      </c>
+      <c r="D123" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="E123" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="F123" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="G123" s="5">
+        <v>11</v>
+      </c>
+      <c r="H123" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="I123" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="J123" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,4935313154</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="3">
+        <v>5021930026</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="C124" s="5">
+        <v>7777777777</v>
+      </c>
+      <c r="D124" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="E124" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="F124" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="G124" s="5">
+        <v>11</v>
+      </c>
+      <c r="H124" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="I124" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="J124" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,5021930026</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="3">
+        <v>5022445212</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="C125" s="5">
+        <v>6666666666</v>
+      </c>
+      <c r="D125" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="E125" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="F125" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="G125" s="5">
+        <v>11</v>
+      </c>
+      <c r="H125" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="I125" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="J125" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,5022445212</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="3">
+        <v>5058885376</v>
+      </c>
+      <c r="B126" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="C126" s="5">
+        <v>5555555555</v>
+      </c>
+      <c r="D126" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="E126" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="F126" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="G126" s="5">
+        <v>11</v>
+      </c>
+      <c r="H126" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="I126" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="J126" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>http://www.focustextil.com.br/evento-criciuma-2017/index.html?368,5058885376</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <conditionalFormatting sqref="F86:F120">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F85">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="F52" r:id="rId1"/>

</xml_diff>